<commit_message>
updated the names for the model files for 2013-2014
</commit_message>
<xml_diff>
--- a/data/577 Projects/2013-2014/file list.xlsx
+++ b/data/577 Projects/2013-2014/file list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8196" windowHeight="5640"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,23 +390,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -442,23 +425,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -637,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added the feature to show the json data
</commit_message>
<xml_diff>
--- a/data/577 Projects/2013-2014/file list.xlsx
+++ b/data/577 Projects/2013-2014/file list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8196" windowHeight="5640"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,23 +390,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -442,23 +425,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -637,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remember the files for the models
</commit_message>
<xml_diff>
--- a/data/577 Projects/2013-2014/file list.xlsx
+++ b/data/577 Projects/2013-2014/file list.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>PROJ</t>
   </si>
@@ -118,12 +118,6 @@
     <t>~577projects\fall2013\projects\team16\team16a\Archive\FinalDeliverables\TRR</t>
   </si>
   <si>
-    <t>~577projects\fall2013\projects\team09\team09a\Valuation</t>
-  </si>
-  <si>
-    <t>inside zipfolder(team09a.zip)</t>
-  </si>
-  <si>
     <t>F13a_City_of_LosAngeles_Public_Safety_Applicant_Resource_Center</t>
   </si>
   <si>
@@ -179,6 +173,12 @@
   </si>
   <si>
     <t>S14b_Lose4Good.org_Database_Driven_Socially_Connected_Website</t>
+  </si>
+  <si>
+    <t>~577projects\fall2013\projects\team09\team09a\Valuation(inside zipfolder(team09a.zip)</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,6 +675,9 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
+      <c r="E6">
+        <v>541</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -689,6 +692,9 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
+      <c r="E7">
+        <v>577.6</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -703,6 +709,9 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
+      <c r="E8">
+        <v>912</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -717,34 +726,42 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1193</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1328</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -752,13 +769,16 @@
         <v>3</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="E12" s="8">
+        <v>512</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -766,15 +786,17 @@
         <v>4</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="E13" s="14">
+        <v>432</v>
+      </c>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -782,13 +804,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -796,13 +818,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="E15" s="17">
+        <v>384.56</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -810,28 +835,33 @@
         <v>7</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="23"/>
+        <v>43</v>
+      </c>
+      <c r="E16" s="23">
+        <v>1045.76</v>
+      </c>
     </row>
     <row r="17" spans="1:5" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="26">
         <v>8</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="E17" s="23">
+        <v>1810.32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -842,13 +872,13 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -864,6 +894,9 @@
       <c r="D19" t="s">
         <v>23</v>
       </c>
+      <c r="E19">
+        <v>1393.84</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -878,6 +911,9 @@
       <c r="D20" t="s">
         <v>24</v>
       </c>
+      <c r="E20">
+        <v>1092.8800000000001</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -892,6 +928,9 @@
       <c r="D21" t="s">
         <v>25</v>
       </c>
+      <c r="E21">
+        <v>8224.7199999999993</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -906,6 +945,9 @@
       <c r="D22" t="s">
         <v>27</v>
       </c>
+      <c r="E22">
+        <v>1741.92</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -920,6 +962,9 @@
       <c r="D23" t="s">
         <v>28</v>
       </c>
+      <c r="E23">
+        <v>950</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -934,6 +979,9 @@
       <c r="D24" t="s">
         <v>31</v>
       </c>
+      <c r="E24">
+        <v>1295.04</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -947,6 +995,9 @@
       </c>
       <c r="D25" t="s">
         <v>33</v>
+      </c>
+      <c r="E25">
+        <v>1506.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the use case to the models for year 2013-2014
</commit_message>
<xml_diff>
--- a/data/577 Projects/2013-2014/file list.xlsx
+++ b/data/577 Projects/2013-2014/file list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8196" windowHeight="5640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5970" windowHeight="5640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,18 +604,18 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="35.21875" customWidth="1"/>
-    <col min="4" max="4" width="79.5546875" customWidth="1"/>
-    <col min="5" max="5" width="64.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="79.5703125" customWidth="1"/>
+    <col min="5" max="5" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -631,7 +631,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -648,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -662,7 +662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -679,7 +679,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -696,7 +696,7 @@
         <v>577.6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -713,7 +713,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -730,7 +730,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -747,7 +747,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>2</v>
       </c>
@@ -764,7 +764,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>3</v>
       </c>
@@ -781,7 +781,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>4</v>
       </c>
@@ -799,7 +799,7 @@
       </c>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>5</v>
       </c>
@@ -813,7 +813,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>6</v>
       </c>
@@ -830,7 +830,7 @@
         <v>384.56</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>7</v>
       </c>
@@ -847,7 +847,7 @@
         <v>1045.76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="26">
         <v>8</v>
       </c>
@@ -864,7 +864,7 @@
         <v>1810.32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -881,7 +881,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -898,7 +898,7 @@
         <v>1393.84</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
@@ -915,7 +915,7 @@
         <v>1092.8800000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -932,7 +932,7 @@
         <v>8224.7199999999993</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -949,7 +949,7 @@
         <v>1741.92</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14</v>
       </c>
@@ -966,7 +966,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -983,7 +983,7 @@
         <v>1295.04</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
created script to transfer the original database to new structure
</commit_message>
<xml_diff>
--- a/data/577 Projects/2013-2014/file list.xlsx
+++ b/data/577 Projects/2013-2014/file list.xlsx
@@ -610,14 +610,14 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>